<commit_message>
Cambios en los casos de prueba
</commit_message>
<xml_diff>
--- a/Casos de prueba/TC-2.xlsx
+++ b/Casos de prueba/TC-2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seba/Documents/GitHub/TestingAplicaciones-FFC-TPO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seba/Documents/GitHub/TestingAplicaciones-FFC-TPO/Casos de prueba/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDA76F1-D04A-6747-B8BB-45ACC6AE580E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC14F2F9-9E63-B34C-907F-67D7AEBBE653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{DCE1F527-8622-40D5-806A-6A7E2BCE07A3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -212,9 +212,6 @@
     <t>register user</t>
   </si>
   <si>
-    <t xml:space="preserve">18 &lt; user </t>
-  </si>
-  <si>
     <t>Test Registration Functionality in Banking</t>
   </si>
   <si>
@@ -222,6 +219,15 @@
   </si>
   <si>
     <t>First name: cami</t>
+  </si>
+  <si>
+    <t>Agrergar los datos requeridos</t>
+  </si>
+  <si>
+    <t>Resultado esperado del registro de user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 &lt;= user </t>
   </si>
 </sst>
 </file>
@@ -239,6 +245,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -647,7 +654,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -742,24 +749,81 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -769,61 +833,16 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="21" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1147,12 +1166,12 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1167,10 +1186,10 @@
       <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="33"/>
+      <c r="D1" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="56"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -1180,23 +1199,23 @@
       <c r="C2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="47"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="3" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="42" t="s">
+      <c r="C3" s="53"/>
+      <c r="D3" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="33">
         <v>2.1</v>
       </c>
       <c r="F3" s="1"/>
@@ -1259,7 +1278,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="24" x14ac:dyDescent="0.2">
@@ -1281,13 +1300,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D9" s="4">
         <v>4</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -1389,26 +1408,28 @@
       <c r="A22" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="53"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="25"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="56"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="46"/>
     </row>
     <row r="24" spans="1:14" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="49"/>
+      <c r="B24" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="48"/>
       <c r="D24" s="19" t="s">
         <v>18</v>
       </c>
@@ -1417,19 +1438,19 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="38" t="s">
+      <c r="G25" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="40"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="59"/>
     </row>
     <row r="26" spans="1:14" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
@@ -1443,62 +1464,62 @@
         <v>29</v>
       </c>
       <c r="E26" s="29"/>
-      <c r="G26" s="36" t="s">
+      <c r="G26" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="H26" s="37"/>
-      <c r="I26" s="36" t="s">
+      <c r="H26" s="50"/>
+      <c r="I26" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="J26" s="37"/>
-      <c r="K26" s="36" t="s">
+      <c r="J26" s="50"/>
+      <c r="K26" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="L26" s="37"/>
-      <c r="M26" s="36" t="s">
+      <c r="L26" s="50"/>
+      <c r="M26" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="N26" s="37"/>
+      <c r="N26" s="50"/>
     </row>
     <row r="27" spans="1:14" ht="47" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>1</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="34" t="s">
+      <c r="C27" s="38"/>
+      <c r="D27" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="35"/>
-      <c r="G27" s="36" t="s">
+      <c r="E27" s="38"/>
+      <c r="G27" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="H27" s="37"/>
-      <c r="I27" s="36" t="s">
+      <c r="H27" s="50"/>
+      <c r="I27" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="36" t="s">
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="N27" s="37"/>
+      <c r="N27" s="50"/>
     </row>
     <row r="28" spans="1:14" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15">
         <v>2</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="34" t="s">
+      <c r="C28" s="38"/>
+      <c r="D28" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="35"/>
+      <c r="E28" s="38"/>
       <c r="G28" s="11" t="s">
         <v>30</v>
       </c>
@@ -1528,12 +1549,12 @@
       <c r="A29" s="15">
         <v>3</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="35"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="38"/>
       <c r="G29" s="13" t="s">
         <v>34</v>
       </c>
@@ -1561,12 +1582,12 @@
       <c r="A30" s="15">
         <v>4</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="35"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="35"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="38"/>
       <c r="G30" s="13" t="s">
         <v>34</v>
       </c>
@@ -1594,12 +1615,12 @@
       <c r="A31" s="15">
         <v>5</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="58"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="35"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="38"/>
       <c r="G31" s="13" t="s">
         <v>34</v>
       </c>
@@ -1624,6 +1645,15 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="60">
+        <v>6</v>
+      </c>
+      <c r="B32" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="61"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="63"/>
       <c r="G32" s="5"/>
       <c r="H32" s="3"/>
       <c r="I32" s="5"/>
@@ -1654,11 +1684,11 @@
       <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="50"/>
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G36" s="27" t="s">
@@ -1731,31 +1761,33 @@
       <c r="N41" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B35:C35"/>
+  <mergeCells count="26">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G25:N25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B22:E23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B30:C30"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G25:N25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1763,15 +1795,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F6A5A8B846BB61408BAC96912A48B9A8" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e2efab9668351af1ee38b12b0ffd9ede">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2835a775-56e5-473e-93b2-b8b6176d193a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2647aa4c78d06f7c1205c6a6e1c2c79d" ns2:_="">
     <xsd:import namespace="2835a775-56e5-473e-93b2-b8b6176d193a"/>
@@ -1903,6 +1926,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1910,14 +1942,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCD417DE-AE4D-4310-B006-24C26EFB9650}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A3F87F2-577F-4B65-8FEE-A540B5E93770}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1935,6 +1959,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCD417DE-AE4D-4310-B006-24C26EFB9650}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86567253-966F-4F1D-B2AE-0608F592F601}">
   <ds:schemaRefs>

</xml_diff>